<commit_message>
added analysis using WHO data
</commit_message>
<xml_diff>
--- a/covid19_dataset.xlsx
+++ b/covid19_dataset.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="243">
   <si>
     <t>Country Name</t>
   </si>
@@ -31,10 +31,13 @@
     <t>United States</t>
   </si>
   <si>
+    <t>India</t>
+  </si>
+  <si>
     <t>Brazil</t>
   </si>
   <si>
-    <t>India</t>
+    <t>France</t>
   </si>
   <si>
     <t>Russia</t>
@@ -43,7 +46,7 @@
     <t>United Kingdom</t>
   </si>
   <si>
-    <t>France</t>
+    <t>Turkey</t>
   </si>
   <si>
     <t>Italy</t>
@@ -52,39 +55,36 @@
     <t>Spain</t>
   </si>
   <si>
-    <t>Turkey</t>
-  </si>
-  <si>
     <t>Germany</t>
   </si>
   <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
     <t>Colombia</t>
   </si>
   <si>
-    <t>Argentina</t>
-  </si>
-  <si>
     <t>Mexico</t>
   </si>
   <si>
-    <t>Poland</t>
-  </si>
-  <si>
     <t>Iran</t>
   </si>
   <si>
     <t>Ukraine</t>
   </si>
   <si>
+    <t>Peru</t>
+  </si>
+  <si>
+    <t>Czech Republic</t>
+  </si>
+  <si>
     <t>South Africa</t>
   </si>
   <si>
-    <t>Czech Republic</t>
-  </si>
-  <si>
-    <t>Peru</t>
-  </si>
-  <si>
     <t>Indonesia</t>
   </si>
   <si>
@@ -100,103 +100,115 @@
     <t>Romania</t>
   </si>
   <si>
+    <t>Iraq</t>
+  </si>
+  <si>
     <t>Belgium</t>
   </si>
   <si>
+    <t>Philippines</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
     <t>Israel</t>
   </si>
   <si>
     <t>Portugal</t>
   </si>
   <si>
-    <t>Iraq</t>
-  </si>
-  <si>
-    <t>Sweden</t>
-  </si>
-  <si>
-    <t>Philippines</t>
-  </si>
-  <si>
     <t>Pakistan</t>
   </si>
   <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Serbia</t>
+  </si>
+  <si>
     <t>Switzerland</t>
   </si>
   <si>
-    <t>Bangladesh</t>
-  </si>
-  <si>
-    <t>Hungary</t>
-  </si>
-  <si>
-    <t>Serbia</t>
-  </si>
-  <si>
-    <t>Jordan</t>
-  </si>
-  <si>
     <t>Austria</t>
   </si>
   <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Lebanon</t>
+  </si>
+  <si>
     <t>Morocco</t>
   </si>
   <si>
-    <t>Japan</t>
-  </si>
-  <si>
     <t>United Arab Emirates</t>
   </si>
   <si>
-    <t>Lebanon</t>
-  </si>
-  <si>
     <t>Saudi Arabia</t>
   </si>
   <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>Slovakia</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
     <t>Panama</t>
   </si>
   <si>
-    <t>Slovakia</t>
-  </si>
-  <si>
-    <t>Malaysia</t>
-  </si>
-  <si>
     <t>Ecuador</t>
   </si>
   <si>
     <t>Belarus</t>
   </si>
   <si>
-    <t>Bulgaria</t>
+    <t>Croatia</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>Azerbaijan</t>
   </si>
   <si>
     <t>Georgia</t>
   </si>
   <si>
+    <t>Bolivia</t>
+  </si>
+  <si>
+    <t>Kazakhstan</t>
+  </si>
+  <si>
     <t>Nepal</t>
   </si>
   <si>
-    <t>Bolivia</t>
-  </si>
-  <si>
-    <t>Croatia</t>
+    <t>Tunisia</t>
+  </si>
+  <si>
+    <t>Palestine</t>
   </si>
   <si>
     <t>Dominican Republic</t>
   </si>
   <si>
-    <t>Azerbaijan</t>
-  </si>
-  <si>
-    <t>Tunisia</t>
-  </si>
-  <si>
-    <t>Greece</t>
-  </si>
-  <si>
-    <t>Kazakhstan</t>
+    <t>Kuwait</t>
+  </si>
+  <si>
+    <t>Paraguay</t>
+  </si>
+  <si>
+    <t>Moldova</t>
   </si>
   <si>
     <t>Ireland</t>
@@ -205,36 +217,24 @@
     <t>Denmark</t>
   </si>
   <si>
-    <t>Palestine</t>
-  </si>
-  <si>
-    <t>Kuwait</t>
-  </si>
-  <si>
-    <t>Moldova</t>
+    <t>Ethiopia</t>
+  </si>
+  <si>
+    <t>Lithuania</t>
+  </si>
+  <si>
+    <t>Slovenia</t>
   </si>
   <si>
     <t>Costa Rica</t>
   </si>
   <si>
-    <t>Lithuania</t>
-  </si>
-  <si>
-    <t>Slovenia</t>
-  </si>
-  <si>
     <t>Egypt</t>
   </si>
   <si>
-    <t>Paraguay</t>
-  </si>
-  <si>
     <t>Guatemala</t>
   </si>
   <si>
-    <t>Ethiopia</t>
-  </si>
-  <si>
     <t>Armenia</t>
   </si>
   <si>
@@ -244,76 +244,79 @@
     <t>Qatar</t>
   </si>
   <si>
+    <t>Bosnia and Herzegovina</t>
+  </si>
+  <si>
+    <t>Venezuela</t>
+  </si>
+  <si>
+    <t>Oman</t>
+  </si>
+  <si>
+    <t>Libya</t>
+  </si>
+  <si>
     <t>Nigeria</t>
   </si>
   <si>
-    <t>Bosnia and Herzegovina</t>
-  </si>
-  <si>
-    <t>Oman</t>
-  </si>
-  <si>
-    <t>Libya</t>
-  </si>
-  <si>
-    <t>Venezuela</t>
+    <t>Bahrain</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>North Macedonia</t>
   </si>
   <si>
     <t>Myanmar</t>
   </si>
   <si>
-    <t>Bahrain</t>
-  </si>
-  <si>
     <t>Albania</t>
   </si>
   <si>
-    <t>Kenya</t>
-  </si>
-  <si>
-    <t>North Macedonia</t>
-  </si>
-  <si>
     <t>Algeria</t>
   </si>
   <si>
+    <t>Estonia</t>
+  </si>
+  <si>
     <t>South Korea</t>
   </si>
   <si>
     <t>Latvia</t>
   </si>
   <si>
-    <t>Estonia</t>
+    <t>Norway</t>
   </si>
   <si>
     <t>Puerto Rico</t>
   </si>
   <si>
+    <t>Kosovo</t>
+  </si>
+  <si>
     <t>Sri Lanka</t>
   </si>
   <si>
+    <t>Montenegro</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>Kyrgyzstan</t>
+  </si>
+  <si>
+    <t>Zambia</t>
+  </si>
+  <si>
     <t>China</t>
   </si>
   <si>
-    <t>Ghana</t>
-  </si>
-  <si>
-    <t>Montenegro</t>
-  </si>
-  <si>
-    <t>Norway</t>
-  </si>
-  <si>
-    <t>Kyrgyzstan</t>
-  </si>
-  <si>
-    <t>Zambia</t>
-  </si>
-  <si>
-    <t>Kosovo</t>
-  </si>
-  <si>
-    <t>Uruguay</t>
+    <t>Cuba</t>
   </si>
   <si>
     <t>Uzbekistan</t>
@@ -325,28 +328,40 @@
     <t>Mozambique</t>
   </si>
   <si>
-    <t>Cuba</t>
-  </si>
-  <si>
     <t>El Salvador</t>
   </si>
   <si>
+    <t>Luxembourg</t>
+  </si>
+  <si>
+    <t>Cameroon</t>
+  </si>
+  <si>
     <t>Singapore</t>
   </si>
   <si>
-    <t>Luxembourg</t>
-  </si>
-  <si>
     <t>Afghanistan</t>
   </si>
   <si>
+    <t>Cyprus</t>
+  </si>
+  <si>
     <t>Namibia</t>
   </si>
   <si>
+    <t>Ivory Coast</t>
+  </si>
+  <si>
+    <t>Jamaica</t>
+  </si>
+  <si>
     <t>Uganda</t>
   </si>
   <si>
-    <t>Cyprus</t>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>Botswana</t>
   </si>
   <si>
     <t>Senegal</t>
@@ -355,123 +370,120 @@
     <t>Zimbabwe</t>
   </si>
   <si>
-    <t>Cameroon</t>
-  </si>
-  <si>
-    <t>Ivory Coast</t>
-  </si>
-  <si>
     <t>Malawi</t>
   </si>
   <si>
-    <t>Botswana</t>
-  </si>
-  <si>
-    <t>Jamaica</t>
+    <t>Sudan</t>
+  </si>
+  <si>
+    <t>Malta</t>
   </si>
   <si>
     <t>Australia</t>
   </si>
   <si>
-    <t>Malta</t>
-  </si>
-  <si>
-    <t>Sudan</t>
-  </si>
-  <si>
-    <t>Thailand</t>
+    <t>Madagascar</t>
   </si>
   <si>
     <t>DR Congo</t>
   </si>
   <si>
+    <t>Maldives</t>
+  </si>
+  <si>
     <t>Donetsk PR</t>
   </si>
   <si>
-    <t>Maldives</t>
-  </si>
-  <si>
-    <t>Madagascar</t>
-  </si>
-  <si>
     <t>Angola</t>
   </si>
   <si>
     <t>Rwanda</t>
   </si>
   <si>
+    <t>Gabon</t>
+  </si>
+  <si>
+    <t>Guinea</t>
+  </si>
+  <si>
+    <t>Syria</t>
+  </si>
+  <si>
+    <t>Cape Verde</t>
+  </si>
+  <si>
+    <t>Mongolia</t>
+  </si>
+  <si>
     <t>French Polynesia</t>
   </si>
   <si>
-    <t>Guinea</t>
-  </si>
-  <si>
-    <t>Gabon</t>
-  </si>
-  <si>
     <t>Mauritania</t>
   </si>
   <si>
     <t>Eswatini</t>
   </si>
   <si>
-    <t>Syria</t>
-  </si>
-  <si>
-    <t>Cape Verde</t>
-  </si>
-  <si>
     <t>Tajikistan</t>
   </si>
   <si>
     <t>Abkhazia</t>
   </si>
   <si>
+    <t>Somalia</t>
+  </si>
+  <si>
     <t>Haiti</t>
   </si>
   <si>
+    <t>Andorra</t>
+  </si>
+  <si>
+    <t>Belize</t>
+  </si>
+  <si>
     <t>Burkina Faso</t>
   </si>
   <si>
-    <t>Belize</t>
-  </si>
-  <si>
-    <t>Andorra</t>
+    <t>Togo</t>
+  </si>
+  <si>
+    <t>Curaçao</t>
   </si>
   <si>
     <t>Hong Kong</t>
   </si>
   <si>
+    <t>Guyana</t>
+  </si>
+  <si>
+    <t>Mali</t>
+  </si>
+  <si>
     <t>Lesotho</t>
   </si>
   <si>
-    <t>Somalia</t>
-  </si>
-  <si>
     <t>South Sudan</t>
   </si>
   <si>
-    <t>Guyana</t>
+    <t>Aruba</t>
   </si>
   <si>
     <t>Congo</t>
   </si>
   <si>
-    <t>Mali</t>
+    <t>Djibouti</t>
   </si>
   <si>
     <t>Suriname</t>
   </si>
   <si>
-    <t>Togo</t>
-  </si>
-  <si>
-    <t>Aruba</t>
-  </si>
-  <si>
     <t>Bahamas</t>
   </si>
   <si>
+    <t>Papua New Guinea</t>
+  </si>
+  <si>
     <t>Trinidad and Tobago</t>
   </si>
   <si>
@@ -487,58 +499,55 @@
     <t>Nicaragua</t>
   </si>
   <si>
-    <t>Djibouti</t>
-  </si>
-  <si>
     <t>Iceland</t>
   </si>
   <si>
-    <t>Curaçao</t>
+    <t>Cambodia</t>
+  </si>
+  <si>
+    <t>Central African Republic</t>
+  </si>
+  <si>
+    <t>Yemen</t>
   </si>
   <si>
     <t>The Gambia</t>
   </si>
   <si>
-    <t>Central African Republic</t>
+    <t>San Marino</t>
+  </si>
+  <si>
+    <t>Seychelles</t>
   </si>
   <si>
     <t>Niger</t>
   </si>
   <si>
-    <t>Mongolia</t>
-  </si>
-  <si>
-    <t>San Marino</t>
+    <t>Chad</t>
+  </si>
+  <si>
+    <t>Saint Lucia</t>
   </si>
   <si>
     <t>Gibraltar</t>
   </si>
   <si>
-    <t>Chad</t>
-  </si>
-  <si>
-    <t>Saint Lucia</t>
-  </si>
-  <si>
     <t>Sierra Leone</t>
   </si>
   <si>
     <t>Northern Cyprus</t>
   </si>
   <si>
-    <t>Seychelles</t>
+    <t>Barbados</t>
+  </si>
+  <si>
+    <t>Guinea-Bissau</t>
   </si>
   <si>
     <t>Comoros</t>
   </si>
   <si>
-    <t>Guinea-Bissau</t>
-  </si>
-  <si>
-    <t>Barbados</t>
-  </si>
-  <si>
-    <t>Yemen</t>
+    <t>Burundi</t>
   </si>
   <si>
     <t>Jersey</t>
@@ -547,69 +556,72 @@
     <t>Luhansk PR</t>
   </si>
   <si>
+    <t>Eritrea</t>
+  </si>
+  <si>
     <t>South Ossetia</t>
   </si>
   <si>
     <t>U.S. Virgin Islands</t>
   </si>
   <si>
-    <t>Papua New Guinea</t>
-  </si>
-  <si>
     <t>Liechtenstein</t>
   </si>
   <si>
-    <t>Burundi</t>
-  </si>
-  <si>
     <t>Vietnam</t>
   </si>
   <si>
     <t>Artsakh</t>
   </si>
   <si>
-    <t>Eritrea</t>
-  </si>
-  <si>
     <t>Turks and Caicos Islands</t>
   </si>
   <si>
     <t>São Tomé and Príncipe</t>
   </si>
   <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
     <t>Sint Maarten</t>
   </si>
   <si>
-    <t>New Zealand</t>
-  </si>
-  <si>
     <t>Liberia</t>
   </si>
   <si>
     <t>Monaco</t>
   </si>
   <si>
+    <t>Bermuda</t>
+  </si>
+  <si>
     <t>Somaliland</t>
   </si>
   <si>
-    <t>Cambodia</t>
-  </si>
-  <si>
     <t>Saint Vincent and The Grenadines</t>
   </si>
   <si>
+    <t>Isle of Man</t>
+  </si>
+  <si>
+    <t>Bonaire</t>
+  </si>
+  <si>
+    <t>East Timor</t>
+  </si>
+  <si>
+    <t>Antigua and Barbuda</t>
+  </si>
+  <si>
+    <t>Mauritius</t>
+  </si>
+  <si>
     <t>USS Theodore Roosevelt</t>
   </si>
   <si>
-    <t>Isle of Man</t>
-  </si>
-  <si>
     <t>Charles de Gaulle</t>
   </si>
   <si>
-    <t>Antigua and Barbuda</t>
-  </si>
-  <si>
     <t>Taiwan</t>
   </si>
   <si>
@@ -619,37 +631,28 @@
     <t>Guernsey</t>
   </si>
   <si>
-    <t>Bermuda</t>
-  </si>
-  <si>
     <t>Diamond Princess</t>
   </si>
   <si>
     <t>Faroe Islands</t>
   </si>
   <si>
-    <t>Mauritius</t>
-  </si>
-  <si>
-    <t>Bonaire</t>
-  </si>
-  <si>
     <t>Cayman Islands</t>
   </si>
   <si>
-    <t>East Timor</t>
-  </si>
-  <si>
     <t>Wallis and Futuna</t>
   </si>
   <si>
     <t>Brunei</t>
   </si>
   <si>
+    <t>Dominica</t>
+  </si>
+  <si>
     <t>Northern Mariana Islands</t>
   </si>
   <si>
-    <t>Dominica</t>
+    <t>Grenada</t>
   </si>
   <si>
     <t>British Virgin Islands</t>
@@ -658,9 +661,6 @@
     <t>Costa Atlantica</t>
   </si>
   <si>
-    <t>Grenada</t>
-  </si>
-  <si>
     <t>Greg Mortimer</t>
   </si>
   <si>
@@ -670,12 +670,12 @@
     <t>Fiji</t>
   </si>
   <si>
+    <t>Falkland Islands</t>
+  </si>
+  <si>
     <t>Antarctica</t>
   </si>
   <si>
-    <t>Falkland Islands</t>
-  </si>
-  <si>
     <t>Laos</t>
   </si>
   <si>
@@ -694,12 +694,12 @@
     <t>Vatican City</t>
   </si>
   <si>
+    <t>Anguilla</t>
+  </si>
+  <si>
     <t>Saint Pierre and Miquelon</t>
   </si>
   <si>
-    <t>Anguilla</t>
-  </si>
-  <si>
     <t>Montserrat</t>
   </si>
   <si>
@@ -722,6 +722,9 @@
   </si>
   <si>
     <t>Saba</t>
+  </si>
+  <si>
+    <t>Saint Helena, Ascension and Tristan da Cunha</t>
   </si>
   <si>
     <t>Marshall Islands</t>
@@ -1097,7 +1100,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E239"/>
+  <dimension ref="A1:E240"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1125,10 +1128,10 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>30054603</v>
+        <v>31764754</v>
       </c>
       <c r="D2">
-        <v>548171</v>
+        <v>571464</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1142,13 +1145,13 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>11998233</v>
+        <v>14291917</v>
       </c>
       <c r="D3">
-        <v>294115</v>
+        <v>174308</v>
       </c>
       <c r="E3">
-        <v>10449933</v>
+        <v>12547866</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1159,13 +1162,13 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>11599130</v>
+        <v>13834342</v>
       </c>
       <c r="D4">
-        <v>159755</v>
+        <v>369024</v>
       </c>
       <c r="E4">
-        <v>11130288</v>
+        <v>12298863</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1176,13 +1179,13 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>4466153</v>
+        <v>5224321</v>
       </c>
       <c r="D5">
-        <v>95391</v>
+        <v>100404</v>
       </c>
       <c r="E5">
-        <v>4077185</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1193,13 +1196,13 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>4291271</v>
+        <v>4693469</v>
       </c>
       <c r="D6">
-        <v>126122</v>
+        <v>105193</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>4319389</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1210,10 +1213,10 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>4252022</v>
+        <v>4380976</v>
       </c>
       <c r="D7">
-        <v>92167</v>
+        <v>127191</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1227,13 +1230,13 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>3356331</v>
+        <v>4150039</v>
       </c>
       <c r="D8">
-        <v>104642</v>
+        <v>35320</v>
       </c>
       <c r="E8">
-        <v>2686236</v>
+        <v>3591550</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1244,13 +1247,13 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>3212332</v>
+        <v>3826156</v>
       </c>
       <c r="D9">
-        <v>72910</v>
+        <v>115937</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>3200196</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1261,13 +1264,13 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>3013122</v>
+        <v>3407283</v>
       </c>
       <c r="D10">
-        <v>30061</v>
+        <v>76981</v>
       </c>
       <c r="E10">
-        <v>2825187</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1278,13 +1281,13 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>2658851</v>
+        <v>3095016</v>
       </c>
       <c r="D11">
-        <v>75196</v>
+        <v>80141</v>
       </c>
       <c r="E11">
-        <v>2409360</v>
+        <v>2735748</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1295,13 +1298,13 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>2331187</v>
+        <v>2675874</v>
       </c>
       <c r="D12">
-        <v>61907</v>
+        <v>61825</v>
       </c>
       <c r="E12">
-        <v>2225725</v>
+        <v>2285221</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1312,13 +1315,13 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>2241686</v>
+        <v>2658574</v>
       </c>
       <c r="D13">
-        <v>54517</v>
+        <v>59084</v>
       </c>
       <c r="E13">
-        <v>2023626</v>
+        <v>2324053</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1329,13 +1332,13 @@
         <v>16</v>
       </c>
       <c r="C14">
-        <v>2195772</v>
+        <v>2619422</v>
       </c>
       <c r="D14">
-        <v>198036</v>
+        <v>67564</v>
       </c>
       <c r="E14">
-        <v>1736159</v>
+        <v>2442453</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1346,13 +1349,13 @@
         <v>17</v>
       </c>
       <c r="C15">
-        <v>2073129</v>
+        <v>2299939</v>
       </c>
       <c r="D15">
-        <v>49365</v>
+        <v>211693</v>
       </c>
       <c r="E15">
-        <v>1676008</v>
+        <v>1823732</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1363,13 +1366,13 @@
         <v>18</v>
       </c>
       <c r="C16">
-        <v>1793805</v>
+        <v>2194133</v>
       </c>
       <c r="D16">
-        <v>61724</v>
+        <v>66008</v>
       </c>
       <c r="E16">
-        <v>1536606</v>
+        <v>1761497</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1380,13 +1383,13 @@
         <v>19</v>
       </c>
       <c r="C17">
-        <v>1554256</v>
+        <v>1936228</v>
       </c>
       <c r="D17">
-        <v>30098</v>
+        <v>39536</v>
       </c>
       <c r="E17">
-        <v>1260842</v>
+        <v>1475556</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1397,13 +1400,13 @@
         <v>20</v>
       </c>
       <c r="C18">
-        <v>1537852</v>
+        <v>1689051</v>
       </c>
       <c r="D18">
-        <v>52111</v>
+        <v>56454</v>
       </c>
       <c r="E18">
-        <v>1463089</v>
+        <v>1610563</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1414,13 +1417,13 @@
         <v>21</v>
       </c>
       <c r="C19">
-        <v>1469547</v>
+        <v>1600341</v>
       </c>
       <c r="D19">
-        <v>24667</v>
+        <v>28396</v>
       </c>
       <c r="E19">
-        <v>1253309</v>
+        <v>1495570</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1431,13 +1434,13 @@
         <v>22</v>
       </c>
       <c r="C20">
-        <v>1466326</v>
+        <v>1564355</v>
       </c>
       <c r="D20">
-        <v>50198</v>
+        <v>53663</v>
       </c>
       <c r="E20">
-        <v>1381318</v>
+        <v>1488572</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1448,13 +1451,13 @@
         <v>23</v>
       </c>
       <c r="C21">
-        <v>1465928</v>
+        <v>1599763</v>
       </c>
       <c r="D21">
-        <v>39711</v>
+        <v>43328</v>
       </c>
       <c r="E21">
-        <v>1297967</v>
+        <v>1450192</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1465,10 +1468,10 @@
         <v>24</v>
       </c>
       <c r="C22">
-        <v>1194580</v>
+        <v>1378145</v>
       </c>
       <c r="D22">
-        <v>16260</v>
+        <v>16861</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -1482,13 +1485,13 @@
         <v>25</v>
       </c>
       <c r="C23">
-        <v>931939</v>
+        <v>1109311</v>
       </c>
       <c r="D23">
-        <v>22279</v>
+        <v>24923</v>
       </c>
       <c r="E23">
-        <v>871234</v>
+        <v>1037539</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1499,13 +1502,13 @@
         <v>26</v>
       </c>
       <c r="C24">
-        <v>930516</v>
+        <v>1106062</v>
       </c>
       <c r="D24">
-        <v>22643</v>
+        <v>23541</v>
       </c>
       <c r="E24">
-        <v>873590</v>
+        <v>997202</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1516,13 +1519,13 @@
         <v>27</v>
       </c>
       <c r="C25">
-        <v>900858</v>
+        <v>1027039</v>
       </c>
       <c r="D25">
-        <v>22268</v>
+        <v>26072</v>
       </c>
       <c r="E25">
-        <v>808754</v>
+        <v>936515</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1533,13 +1536,13 @@
         <v>28</v>
       </c>
       <c r="C26">
-        <v>837006</v>
+        <v>956860</v>
       </c>
       <c r="D26">
-        <v>22707</v>
+        <v>14885</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>837336</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1550,13 +1553,13 @@
         <v>29</v>
       </c>
       <c r="C27">
-        <v>827220</v>
+        <v>943213</v>
       </c>
       <c r="D27">
-        <v>6082</v>
+        <v>23681</v>
       </c>
       <c r="E27">
-        <v>802337</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1567,13 +1570,13 @@
         <v>30</v>
       </c>
       <c r="C28">
-        <v>817530</v>
+        <v>914971</v>
       </c>
       <c r="D28">
-        <v>16768</v>
+        <v>15738</v>
       </c>
       <c r="E28">
-        <v>767319</v>
+        <v>705757</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1584,13 +1587,13 @@
         <v>31</v>
       </c>
       <c r="C29">
-        <v>789390</v>
+        <v>900138</v>
       </c>
       <c r="D29">
-        <v>13969</v>
+        <v>13788</v>
       </c>
       <c r="E29">
-        <v>710699</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1601,13 +1604,13 @@
         <v>32</v>
       </c>
       <c r="C30">
-        <v>744272</v>
+        <v>836706</v>
       </c>
       <c r="D30">
-        <v>13262</v>
+        <v>6314</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>827447</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1618,13 +1621,13 @@
         <v>33</v>
       </c>
       <c r="C31">
-        <v>671792</v>
+        <v>829911</v>
       </c>
       <c r="D31">
-        <v>12972</v>
+        <v>16937</v>
       </c>
       <c r="E31">
-        <v>577850</v>
+        <v>787607</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1635,13 +1638,13 @@
         <v>34</v>
       </c>
       <c r="C32">
-        <v>630471</v>
+        <v>750158</v>
       </c>
       <c r="D32">
-        <v>13863</v>
+        <v>16094</v>
       </c>
       <c r="E32">
-        <v>583538</v>
+        <v>654956</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1652,13 +1655,13 @@
         <v>35</v>
       </c>
       <c r="C33">
-        <v>580609</v>
+        <v>746802</v>
       </c>
       <c r="D33">
-        <v>9509</v>
+        <v>24979</v>
       </c>
       <c r="E33">
-        <v>317600</v>
+        <v>450791</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1669,13 +1672,13 @@
         <v>36</v>
       </c>
       <c r="C34">
-        <v>570878</v>
+        <v>715252</v>
       </c>
       <c r="D34">
-        <v>8690</v>
+        <v>10283</v>
       </c>
       <c r="E34">
-        <v>522105</v>
+        <v>608815</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1686,13 +1689,13 @@
         <v>37</v>
       </c>
       <c r="C35">
-        <v>560971</v>
+        <v>679138</v>
       </c>
       <c r="D35">
-        <v>18068</v>
+        <v>8057</v>
       </c>
       <c r="E35">
-        <v>366774</v>
+        <v>621870</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1703,10 +1706,10 @@
         <v>38</v>
       </c>
       <c r="C36">
-        <v>546896</v>
+        <v>657716</v>
       </c>
       <c r="D36">
-        <v>4900</v>
+        <v>5920</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -1720,13 +1723,13 @@
         <v>39</v>
       </c>
       <c r="C37">
-        <v>526666</v>
+        <v>632399</v>
       </c>
       <c r="D37">
-        <v>5788</v>
+        <v>9869</v>
       </c>
       <c r="E37">
-        <v>426754</v>
+        <v>317600</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1737,13 +1740,13 @@
         <v>40</v>
       </c>
       <c r="C38">
-        <v>514153</v>
+        <v>589299</v>
       </c>
       <c r="D38">
-        <v>9074</v>
+        <v>9843</v>
       </c>
       <c r="E38">
-        <v>473357</v>
+        <v>550470</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1754,13 +1757,13 @@
         <v>41</v>
       </c>
       <c r="C39">
-        <v>491463</v>
+        <v>525218</v>
       </c>
       <c r="D39">
-        <v>8763</v>
+        <v>9584</v>
       </c>
       <c r="E39">
-        <v>478870</v>
+        <v>478378</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1771,13 +1774,13 @@
         <v>42</v>
       </c>
       <c r="C40">
-        <v>456781</v>
+        <v>506808</v>
       </c>
       <c r="D40">
-        <v>8835</v>
+        <v>6854</v>
       </c>
       <c r="E40">
-        <v>434274</v>
+        <v>420223</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1788,13 +1791,13 @@
         <v>43</v>
       </c>
       <c r="C41">
-        <v>442226</v>
+        <v>504260</v>
       </c>
       <c r="D41">
-        <v>1445</v>
+        <v>8927</v>
       </c>
       <c r="E41">
-        <v>424840</v>
+        <v>490366</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1805,13 +1808,13 @@
         <v>44</v>
       </c>
       <c r="C42">
-        <v>436575</v>
+        <v>495224</v>
       </c>
       <c r="D42">
-        <v>5715</v>
+        <v>1550</v>
       </c>
       <c r="E42">
-        <v>343099</v>
+        <v>478063</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1822,13 +1825,13 @@
         <v>45</v>
       </c>
       <c r="C43">
-        <v>384653</v>
+        <v>403106</v>
       </c>
       <c r="D43">
-        <v>6602</v>
+        <v>6801</v>
       </c>
       <c r="E43">
-        <v>374135</v>
+        <v>387020</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1839,13 +1842,13 @@
         <v>46</v>
       </c>
       <c r="C44">
-        <v>350991</v>
+        <v>384887</v>
       </c>
       <c r="D44">
-        <v>6044</v>
+        <v>15100</v>
       </c>
       <c r="E44">
-        <v>339565</v>
+        <v>304033</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1856,10 +1859,10 @@
         <v>47</v>
       </c>
       <c r="C45">
-        <v>348869</v>
+        <v>375336</v>
       </c>
       <c r="D45">
-        <v>9044</v>
+        <v>11043</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -1873,13 +1876,13 @@
         <v>48</v>
       </c>
       <c r="C46">
-        <v>334156</v>
+        <v>372859</v>
       </c>
       <c r="D46">
-        <v>1238</v>
+        <v>1370</v>
       </c>
       <c r="E46">
-        <v>318784</v>
+        <v>352395</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1890,13 +1893,13 @@
         <v>49</v>
       </c>
       <c r="C47">
-        <v>312598</v>
+        <v>360249</v>
       </c>
       <c r="D47">
-        <v>16451</v>
+        <v>6185</v>
       </c>
       <c r="E47">
-        <v>271847</v>
+        <v>350134</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1907,13 +1910,13 @@
         <v>50</v>
       </c>
       <c r="C48">
-        <v>310445</v>
+        <v>355964</v>
       </c>
       <c r="D48">
-        <v>2157</v>
+        <v>17528</v>
       </c>
       <c r="E48">
-        <v>301442</v>
+        <v>298604</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1924,13 +1927,13 @@
         <v>51</v>
       </c>
       <c r="C49">
-        <v>303423</v>
+        <v>342923</v>
       </c>
       <c r="D49">
-        <v>12019</v>
+        <v>2413</v>
       </c>
       <c r="E49">
-        <v>234771</v>
+        <v>333373</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1941,13 +1944,13 @@
         <v>52</v>
       </c>
       <c r="C50">
-        <v>277218</v>
+        <v>306225</v>
       </c>
       <c r="D50">
-        <v>3691</v>
+        <v>6523</v>
       </c>
       <c r="E50">
-        <v>269784</v>
+        <v>283418</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1958,13 +1961,13 @@
         <v>53</v>
       </c>
       <c r="C51">
-        <v>276056</v>
+        <v>311033</v>
       </c>
       <c r="D51">
-        <v>3019</v>
+        <v>9330</v>
       </c>
       <c r="E51">
-        <v>272020</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1975,13 +1978,13 @@
         <v>54</v>
       </c>
       <c r="C52">
-        <v>264634</v>
+        <v>296374</v>
       </c>
       <c r="D52">
-        <v>12060</v>
+        <v>4077</v>
       </c>
       <c r="E52">
-        <v>212106</v>
+        <v>260193</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1992,13 +1995,13 @@
         <v>55</v>
       </c>
       <c r="C53">
-        <v>257789</v>
+        <v>292244</v>
       </c>
       <c r="D53">
-        <v>5786</v>
+        <v>3908</v>
       </c>
       <c r="E53">
-        <v>245723</v>
+        <v>279389</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -2009,13 +2012,13 @@
         <v>56</v>
       </c>
       <c r="C54">
-        <v>249463</v>
+        <v>287360</v>
       </c>
       <c r="D54">
-        <v>3272</v>
+        <v>12625</v>
       </c>
       <c r="E54">
-        <v>205697</v>
+        <v>236455</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -2026,13 +2029,13 @@
         <v>57</v>
       </c>
       <c r="C55">
-        <v>246304</v>
+        <v>284173</v>
       </c>
       <c r="D55">
-        <v>3351</v>
+        <v>3288</v>
       </c>
       <c r="E55">
-        <v>232876</v>
+        <v>244517</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -2043,13 +2046,13 @@
         <v>58</v>
       </c>
       <c r="C56">
-        <v>244776</v>
+        <v>282890</v>
       </c>
       <c r="D56">
-        <v>8506</v>
+        <v>3070</v>
       </c>
       <c r="E56">
-        <v>211561</v>
+        <v>274812</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -2060,13 +2063,13 @@
         <v>59</v>
       </c>
       <c r="C57">
-        <v>235611</v>
+        <v>281777</v>
       </c>
       <c r="D57">
-        <v>7421</v>
+        <v>9639</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>232643</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -2077,13 +2080,13 @@
         <v>60</v>
       </c>
       <c r="C58">
-        <v>231698</v>
+        <v>272767</v>
       </c>
       <c r="D58">
-        <v>2917</v>
+        <v>2901</v>
       </c>
       <c r="E58">
-        <v>211127</v>
+        <v>237046</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -2094,13 +2097,13 @@
         <v>61</v>
       </c>
       <c r="C59">
-        <v>230599</v>
+        <v>259639</v>
       </c>
       <c r="D59">
-        <v>4587</v>
+        <v>3405</v>
       </c>
       <c r="E59">
-        <v>0</v>
+        <v>217613</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -2111,13 +2114,13 @@
         <v>62</v>
       </c>
       <c r="C60">
-        <v>224258</v>
+        <v>254472</v>
       </c>
       <c r="D60">
-        <v>2397</v>
+        <v>1436</v>
       </c>
       <c r="E60">
-        <v>212580</v>
+        <v>237667</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -2128,13 +2131,13 @@
         <v>63</v>
       </c>
       <c r="C61">
-        <v>221391</v>
+        <v>246806</v>
       </c>
       <c r="D61">
-        <v>2406</v>
+        <v>5177</v>
       </c>
       <c r="E61">
-        <v>196678</v>
+        <v>202109</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -2145,13 +2148,13 @@
         <v>64</v>
       </c>
       <c r="C62">
-        <v>219125</v>
+        <v>244866</v>
       </c>
       <c r="D62">
-        <v>1226</v>
+        <v>5521</v>
       </c>
       <c r="E62">
-        <v>203539</v>
+        <v>228766</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -2162,13 +2165,13 @@
         <v>65</v>
       </c>
       <c r="C63">
-        <v>215034</v>
+        <v>242819</v>
       </c>
       <c r="D63">
-        <v>4559</v>
+        <v>4831</v>
       </c>
       <c r="E63">
-        <v>188363</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -2179,13 +2182,13 @@
         <v>66</v>
       </c>
       <c r="C64">
-        <v>211903</v>
+        <v>241007</v>
       </c>
       <c r="D64">
-        <v>2896</v>
+        <v>2452</v>
       </c>
       <c r="E64">
-        <v>190236</v>
+        <v>230084</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -2196,13 +2199,13 @@
         <v>67</v>
       </c>
       <c r="C65">
-        <v>209340</v>
+        <v>238527</v>
       </c>
       <c r="D65">
-        <v>3486</v>
+        <v>3300</v>
       </c>
       <c r="E65">
-        <v>194345</v>
+        <v>177629</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -2213,13 +2216,13 @@
         <v>68</v>
       </c>
       <c r="C66">
-        <v>206026</v>
+        <v>232829</v>
       </c>
       <c r="D66">
-        <v>3972</v>
+        <v>3751</v>
       </c>
       <c r="E66">
-        <v>0</v>
+        <v>211306</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -2230,13 +2233,13 @@
         <v>69</v>
       </c>
       <c r="C67">
-        <v>195418</v>
+        <v>229966</v>
       </c>
       <c r="D67">
-        <v>11598</v>
+        <v>4142</v>
       </c>
       <c r="E67">
-        <v>149934</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -2247,13 +2250,13 @@
         <v>70</v>
       </c>
       <c r="C68">
-        <v>194122</v>
+        <v>228577</v>
       </c>
       <c r="D68">
-        <v>3730</v>
+        <v>3071</v>
       </c>
       <c r="E68">
-        <v>159774</v>
+        <v>196974</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -2264,13 +2267,13 @@
         <v>71</v>
       </c>
       <c r="C69">
-        <v>187659</v>
+        <v>214639</v>
       </c>
       <c r="D69">
-        <v>6685</v>
+        <v>12653</v>
       </c>
       <c r="E69">
-        <v>171080</v>
+        <v>162170</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -2281,13 +2284,13 @@
         <v>72</v>
       </c>
       <c r="C70">
-        <v>187365</v>
+        <v>210667</v>
       </c>
       <c r="D70">
-        <v>2659</v>
+        <v>7160</v>
       </c>
       <c r="E70">
-        <v>147452</v>
+        <v>189536</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -2298,13 +2301,13 @@
         <v>73</v>
       </c>
       <c r="C71">
-        <v>183713</v>
+        <v>206142</v>
       </c>
       <c r="D71">
-        <v>3348</v>
+        <v>3817</v>
       </c>
       <c r="E71">
-        <v>168289</v>
+        <v>185125</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -2315,13 +2318,13 @@
         <v>74</v>
       </c>
       <c r="C72">
-        <v>182409</v>
+        <v>199682</v>
       </c>
       <c r="D72">
-        <v>4443</v>
+        <v>4934</v>
       </c>
       <c r="E72">
-        <v>69105</v>
+        <v>76235</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -2332,13 +2335,13 @@
         <v>75</v>
       </c>
       <c r="C73">
-        <v>173709</v>
+        <v>194940</v>
       </c>
       <c r="D73">
-        <v>273</v>
+        <v>367</v>
       </c>
       <c r="E73">
-        <v>160451</v>
+        <v>172598</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -2349,13 +2352,13 @@
         <v>76</v>
       </c>
       <c r="C74">
-        <v>161737</v>
+        <v>188994</v>
       </c>
       <c r="D74">
-        <v>2030</v>
+        <v>7788</v>
       </c>
       <c r="E74">
-        <v>147899</v>
+        <v>145863</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -2366,13 +2369,13 @@
         <v>77</v>
       </c>
       <c r="C75">
-        <v>151337</v>
+        <v>179365</v>
       </c>
       <c r="D75">
-        <v>5773</v>
+        <v>1853</v>
       </c>
       <c r="E75">
-        <v>123653</v>
+        <v>161820</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -2383,13 +2386,13 @@
         <v>78</v>
       </c>
       <c r="C76">
-        <v>150800</v>
+        <v>176668</v>
       </c>
       <c r="D76">
-        <v>1622</v>
+        <v>1821</v>
       </c>
       <c r="E76">
-        <v>139100</v>
+        <v>156845</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -2400,13 +2403,13 @@
         <v>79</v>
       </c>
       <c r="C77">
-        <v>150341</v>
+        <v>167825</v>
       </c>
       <c r="D77">
-        <v>2487</v>
+        <v>2823</v>
       </c>
       <c r="E77">
-        <v>137073</v>
+        <v>152921</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -2417,13 +2420,13 @@
         <v>80</v>
       </c>
       <c r="C78">
-        <v>150306</v>
+        <v>164147</v>
       </c>
       <c r="D78">
-        <v>1483</v>
+        <v>2061</v>
       </c>
       <c r="E78">
-        <v>140239</v>
+        <v>154304</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -2434,13 +2437,13 @@
         <v>81</v>
       </c>
       <c r="C79">
-        <v>142246</v>
+        <v>160934</v>
       </c>
       <c r="D79">
-        <v>3204</v>
+        <v>574</v>
       </c>
       <c r="E79">
-        <v>131763</v>
+        <v>149159</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -2451,13 +2454,13 @@
         <v>82</v>
       </c>
       <c r="C80">
-        <v>128428</v>
+        <v>159569</v>
       </c>
       <c r="D80">
-        <v>476</v>
+        <v>1788</v>
       </c>
       <c r="E80">
-        <v>121776</v>
+        <v>126119</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -2468,13 +2471,13 @@
         <v>83</v>
       </c>
       <c r="C81">
-        <v>121200</v>
+        <v>150260</v>
       </c>
       <c r="D81">
-        <v>2137</v>
+        <v>2443</v>
       </c>
       <c r="E81">
-        <v>85147</v>
+        <v>100980</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -2485,13 +2488,13 @@
         <v>84</v>
       </c>
       <c r="C82">
-        <v>120910</v>
+        <v>145909</v>
       </c>
       <c r="D82">
-        <v>2011</v>
+        <v>4388</v>
       </c>
       <c r="E82">
-        <v>89622</v>
+        <v>121439</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -2502,13 +2505,13 @@
         <v>85</v>
       </c>
       <c r="C83">
-        <v>119378</v>
+        <v>142619</v>
       </c>
       <c r="D83">
-        <v>3473</v>
+        <v>3206</v>
       </c>
       <c r="E83">
-        <v>100774</v>
+        <v>131889</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -2519,13 +2522,13 @@
         <v>86</v>
       </c>
       <c r="C84">
-        <v>116066</v>
+        <v>129307</v>
       </c>
       <c r="D84">
-        <v>3055</v>
+        <v>2337</v>
       </c>
       <c r="E84">
-        <v>80566</v>
+        <v>100600</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -2536,13 +2539,13 @@
         <v>87</v>
       </c>
       <c r="C85">
-        <v>99075</v>
+        <v>119323</v>
       </c>
       <c r="D85">
-        <v>1697</v>
+        <v>3148</v>
       </c>
       <c r="E85">
-        <v>90611</v>
+        <v>83169</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -2553,13 +2556,13 @@
         <v>88</v>
       </c>
       <c r="C86">
-        <v>97149</v>
+        <v>117011</v>
       </c>
       <c r="D86">
-        <v>1821</v>
+        <v>1082</v>
       </c>
       <c r="E86">
-        <v>88322</v>
+        <v>101471</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -2570,13 +2573,13 @@
         <v>89</v>
       </c>
       <c r="C87">
-        <v>96394</v>
+        <v>113444</v>
       </c>
       <c r="D87">
-        <v>797</v>
+        <v>1794</v>
       </c>
       <c r="E87">
-        <v>68249</v>
+        <v>103594</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -2587,13 +2590,13 @@
         <v>90</v>
       </c>
       <c r="C88">
-        <v>95762</v>
+        <v>110343</v>
       </c>
       <c r="D88">
-        <v>2096</v>
+        <v>2042</v>
       </c>
       <c r="E88">
-        <v>0</v>
+        <v>101088</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -2604,13 +2607,13 @@
         <v>91</v>
       </c>
       <c r="C89">
-        <v>90200</v>
+        <v>106727</v>
       </c>
       <c r="D89">
-        <v>546</v>
+        <v>708</v>
       </c>
       <c r="E89">
-        <v>86759</v>
+        <v>54004</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -2621,13 +2624,13 @@
         <v>92</v>
       </c>
       <c r="C90">
-        <v>90087</v>
+        <v>105758</v>
       </c>
       <c r="D90">
-        <v>4636</v>
+        <v>2185</v>
       </c>
       <c r="E90">
-        <v>85289</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -2638,13 +2641,13 @@
         <v>93</v>
       </c>
       <c r="C91">
-        <v>89682</v>
+        <v>100655</v>
       </c>
       <c r="D91">
-        <v>725</v>
+        <v>2053</v>
       </c>
       <c r="E91">
-        <v>85761</v>
+        <v>85842</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -2655,13 +2658,13 @@
         <v>94</v>
       </c>
       <c r="C92">
-        <v>87212</v>
+        <v>96186</v>
       </c>
       <c r="D92">
-        <v>1199</v>
+        <v>615</v>
       </c>
       <c r="E92">
-        <v>77914</v>
+        <v>92611</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -2672,13 +2675,13 @@
         <v>95</v>
       </c>
       <c r="C93">
-        <v>86939</v>
+        <v>95205</v>
       </c>
       <c r="D93">
-        <v>648</v>
+        <v>1421</v>
       </c>
       <c r="E93">
-        <v>54004</v>
+        <v>90291</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -2689,13 +2692,13 @@
         <v>96</v>
       </c>
       <c r="C94">
-        <v>86818</v>
+        <v>91260</v>
       </c>
       <c r="D94">
-        <v>1480</v>
+        <v>754</v>
       </c>
       <c r="E94">
-        <v>83809</v>
+        <v>89092</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -2706,13 +2709,13 @@
         <v>97</v>
       </c>
       <c r="C95">
-        <v>86449</v>
+        <v>91144</v>
       </c>
       <c r="D95">
-        <v>1179</v>
+        <v>1540</v>
       </c>
       <c r="E95">
-        <v>83258</v>
+        <v>86491</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -2723,13 +2726,13 @@
         <v>98</v>
       </c>
       <c r="C96">
-        <v>82185</v>
+        <v>90844</v>
       </c>
       <c r="D96">
-        <v>1760</v>
+        <v>1234</v>
       </c>
       <c r="E96">
-        <v>68083</v>
+        <v>88555</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -2740,13 +2743,13 @@
         <v>99</v>
       </c>
       <c r="C97">
-        <v>81537</v>
+        <v>90468</v>
       </c>
       <c r="D97">
-        <v>792</v>
+        <v>4636</v>
       </c>
       <c r="E97">
-        <v>67730</v>
+        <v>85533</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -2757,13 +2760,13 @@
         <v>100</v>
       </c>
       <c r="C98">
-        <v>80247</v>
+        <v>90408</v>
       </c>
       <c r="D98">
-        <v>622</v>
+        <v>491</v>
       </c>
       <c r="E98">
-        <v>78939</v>
+        <v>8512</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -2774,13 +2777,13 @@
         <v>101</v>
       </c>
       <c r="C99">
-        <v>72073</v>
+        <v>85114</v>
       </c>
       <c r="D99">
-        <v>808</v>
+        <v>634</v>
       </c>
       <c r="E99">
-        <v>31000</v>
+        <v>82943</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -2791,13 +2794,13 @@
         <v>102</v>
       </c>
       <c r="C100">
-        <v>66212</v>
+        <v>83633</v>
       </c>
       <c r="D100">
-        <v>746</v>
+        <v>887</v>
       </c>
       <c r="E100">
-        <v>52683</v>
+        <v>31000</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -2808,13 +2811,13 @@
         <v>103</v>
       </c>
       <c r="C101">
-        <v>63725</v>
+        <v>69067</v>
       </c>
       <c r="D101">
-        <v>380</v>
+        <v>797</v>
       </c>
       <c r="E101">
-        <v>59550</v>
+        <v>61188</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -2825,13 +2828,13 @@
         <v>104</v>
       </c>
       <c r="C102">
-        <v>63344</v>
+        <v>67099</v>
       </c>
       <c r="D102">
-        <v>1979</v>
+        <v>2064</v>
       </c>
       <c r="E102">
-        <v>60681</v>
+        <v>63471</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -2842,13 +2845,13 @@
         <v>105</v>
       </c>
       <c r="C103">
-        <v>60184</v>
+        <v>64549</v>
       </c>
       <c r="D103">
-        <v>30</v>
+        <v>785</v>
       </c>
       <c r="E103">
-        <v>60022</v>
+        <v>60563</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -2859,13 +2862,13 @@
         <v>106</v>
       </c>
       <c r="C104">
-        <v>58955</v>
+        <v>61731</v>
       </c>
       <c r="D104">
-        <v>714</v>
+        <v>919</v>
       </c>
       <c r="E104">
-        <v>55147</v>
+        <v>56926</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -2876,13 +2879,13 @@
         <v>107</v>
       </c>
       <c r="C105">
-        <v>56016</v>
+        <v>60653</v>
       </c>
       <c r="D105">
-        <v>2460</v>
+        <v>30</v>
       </c>
       <c r="E105">
-        <v>49536</v>
+        <v>60335</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -2893,13 +2896,13 @@
         <v>108</v>
       </c>
       <c r="C106">
-        <v>41546</v>
+        <v>57242</v>
       </c>
       <c r="D106">
-        <v>477</v>
+        <v>2529</v>
       </c>
       <c r="E106">
-        <v>38942</v>
+        <v>51989</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -2910,13 +2913,13 @@
         <v>109</v>
       </c>
       <c r="C107">
-        <v>40651</v>
+        <v>51505</v>
       </c>
       <c r="D107">
-        <v>334</v>
+        <v>272</v>
       </c>
       <c r="E107">
-        <v>15133</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -2927,13 +2930,13 @@
         <v>110</v>
       </c>
       <c r="C108">
-        <v>40344</v>
+        <v>45527</v>
       </c>
       <c r="D108">
-        <v>241</v>
+        <v>570</v>
       </c>
       <c r="E108">
-        <v>0</v>
+        <v>43640</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -2944,13 +2947,13 @@
         <v>111</v>
       </c>
       <c r="C109">
-        <v>37428</v>
+        <v>45145</v>
       </c>
       <c r="D109">
-        <v>1003</v>
+        <v>261</v>
       </c>
       <c r="E109">
-        <v>33931</v>
+        <v>44473</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -2961,13 +2964,13 @@
         <v>112</v>
       </c>
       <c r="C110">
-        <v>36471</v>
+        <v>42772</v>
       </c>
       <c r="D110">
-        <v>1501</v>
+        <v>676</v>
       </c>
       <c r="E110">
-        <v>34011</v>
+        <v>19132</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -2978,13 +2981,13 @@
         <v>113</v>
       </c>
       <c r="C111">
-        <v>35714</v>
+        <v>41140</v>
       </c>
       <c r="D111">
-        <v>551</v>
+        <v>337</v>
       </c>
       <c r="E111">
-        <v>32594</v>
+        <v>40685</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -2995,13 +2998,13 @@
         <v>114</v>
       </c>
       <c r="C112">
-        <v>34935</v>
+        <v>40585</v>
       </c>
       <c r="D112">
-        <v>200</v>
+        <v>99</v>
       </c>
       <c r="E112">
-        <v>32513</v>
+        <v>28570</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -3012,13 +3015,13 @@
         <v>115</v>
       </c>
       <c r="C113">
-        <v>33237</v>
+        <v>40478</v>
       </c>
       <c r="D113">
-        <v>1096</v>
+        <v>663</v>
       </c>
       <c r="E113">
-        <v>28636</v>
+        <v>38923</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -3029,13 +3032,13 @@
         <v>116</v>
       </c>
       <c r="C114">
-        <v>33107</v>
+        <v>39307</v>
       </c>
       <c r="D114">
-        <v>458</v>
+        <v>1074</v>
       </c>
       <c r="E114">
-        <v>31128</v>
+        <v>38031</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -3046,13 +3049,13 @@
         <v>117</v>
       </c>
       <c r="C115">
-        <v>29912</v>
+        <v>37369</v>
       </c>
       <c r="D115">
-        <v>484</v>
+        <v>1548</v>
       </c>
       <c r="E115">
-        <v>15059</v>
+        <v>34946</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -3063,13 +3066,13 @@
         <v>118</v>
       </c>
       <c r="C116">
-        <v>29183</v>
+        <v>33919</v>
       </c>
       <c r="D116">
-        <v>909</v>
+        <v>1136</v>
       </c>
       <c r="E116">
-        <v>0</v>
+        <v>31717</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -3080,13 +3083,13 @@
         <v>119</v>
       </c>
       <c r="C117">
-        <v>28319</v>
+        <v>31790</v>
       </c>
       <c r="D117">
-        <v>373</v>
+        <v>2208</v>
       </c>
       <c r="E117">
-        <v>25343</v>
+        <v>25539</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -3097,13 +3100,13 @@
         <v>120</v>
       </c>
       <c r="C118">
-        <v>28025</v>
+        <v>29927</v>
       </c>
       <c r="D118">
-        <v>1864</v>
+        <v>409</v>
       </c>
       <c r="E118">
-        <v>22606</v>
+        <v>28910</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -3114,13 +3117,13 @@
         <v>121</v>
       </c>
       <c r="C119">
-        <v>27876</v>
+        <v>29405</v>
       </c>
       <c r="D119">
-        <v>91</v>
+        <v>909</v>
       </c>
       <c r="E119">
-        <v>26663</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -3131,13 +3134,13 @@
         <v>122</v>
       </c>
       <c r="C120">
-        <v>26737</v>
+        <v>29348</v>
       </c>
       <c r="D120">
-        <v>712</v>
+        <v>520</v>
       </c>
       <c r="E120">
-        <v>22432</v>
+        <v>24893</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -3148,13 +3151,13 @@
         <v>123</v>
       </c>
       <c r="C121">
-        <v>25517</v>
+        <v>28859</v>
       </c>
       <c r="D121">
-        <v>2092</v>
+        <v>745</v>
       </c>
       <c r="E121">
-        <v>17280</v>
+        <v>25841</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -3165,13 +3168,13 @@
         <v>124</v>
       </c>
       <c r="C122">
-        <v>22373</v>
+        <v>25701</v>
       </c>
       <c r="D122">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E122">
-        <v>19895</v>
+        <v>22791</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -3182,13 +3185,13 @@
         <v>125</v>
       </c>
       <c r="C123">
-        <v>22113</v>
+        <v>25517</v>
       </c>
       <c r="D123">
-        <v>340</v>
+        <v>2092</v>
       </c>
       <c r="E123">
-        <v>20996</v>
+        <v>17280</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -3199,13 +3202,13 @@
         <v>126</v>
       </c>
       <c r="C124">
-        <v>21696</v>
+        <v>23841</v>
       </c>
       <c r="D124">
-        <v>526</v>
+        <v>557</v>
       </c>
       <c r="E124">
-        <v>20068</v>
+        <v>22144</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -3216,13 +3219,13 @@
         <v>127</v>
       </c>
       <c r="C125">
-        <v>20551</v>
+        <v>23426</v>
       </c>
       <c r="D125">
-        <v>284</v>
+        <v>315</v>
       </c>
       <c r="E125">
-        <v>19007</v>
+        <v>21243</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -3233,13 +3236,13 @@
         <v>128</v>
       </c>
       <c r="C126">
-        <v>18546</v>
+        <v>21566</v>
       </c>
       <c r="D126">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="E126">
-        <v>4842</v>
+        <v>18219</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -3250,13 +3253,13 @@
         <v>129</v>
       </c>
       <c r="C127">
-        <v>18438</v>
+        <v>21106</v>
       </c>
       <c r="D127">
-        <v>107</v>
+        <v>142</v>
       </c>
       <c r="E127">
-        <v>15804</v>
+        <v>18686</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -3267,13 +3270,13 @@
         <v>130</v>
       </c>
       <c r="C128">
-        <v>17711</v>
+        <v>20555</v>
       </c>
       <c r="D128">
-        <v>106</v>
+        <v>1402</v>
       </c>
       <c r="E128">
-        <v>15495</v>
+        <v>14335</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -3284,13 +3287,13 @@
         <v>131</v>
       </c>
       <c r="C129">
-        <v>17542</v>
+        <v>19780</v>
       </c>
       <c r="D129">
-        <v>445</v>
+        <v>188</v>
       </c>
       <c r="E129">
-        <v>16839</v>
+        <v>17802</v>
       </c>
     </row>
     <row r="130" spans="1:5">
@@ -3301,13 +3304,13 @@
         <v>132</v>
       </c>
       <c r="C130">
-        <v>17274</v>
+        <v>19672</v>
       </c>
       <c r="D130">
-        <v>664</v>
+        <v>37</v>
       </c>
       <c r="E130">
-        <v>15981</v>
+        <v>11044</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -3318,13 +3321,13 @@
         <v>133</v>
       </c>
       <c r="C131">
-        <v>17240</v>
+        <v>18652</v>
       </c>
       <c r="D131">
-        <v>1153</v>
+        <v>141</v>
       </c>
       <c r="E131">
-        <v>11503</v>
+        <v>4842</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -3335,13 +3338,13 @@
         <v>134</v>
       </c>
       <c r="C132">
-        <v>16154</v>
+        <v>18066</v>
       </c>
       <c r="D132">
-        <v>157</v>
+        <v>452</v>
       </c>
       <c r="E132">
-        <v>15549</v>
+        <v>17428</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -3352,13 +3355,13 @@
         <v>135</v>
       </c>
       <c r="C133">
-        <v>13308</v>
+        <v>17376</v>
       </c>
       <c r="D133">
-        <v>90</v>
+        <v>669</v>
       </c>
       <c r="E133">
-        <v>13218</v>
+        <v>16645</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -3369,13 +3372,13 @@
         <v>136</v>
       </c>
       <c r="C134">
-        <v>12931</v>
+        <v>13308</v>
       </c>
       <c r="D134">
-        <v>203</v>
+        <v>90</v>
       </c>
       <c r="E134">
-        <v>12390</v>
+        <v>13218</v>
       </c>
     </row>
     <row r="135" spans="1:5">
@@ -3386,13 +3389,13 @@
         <v>137</v>
       </c>
       <c r="C135">
-        <v>12714</v>
+        <v>12931</v>
       </c>
       <c r="D135">
-        <v>251</v>
+        <v>203</v>
       </c>
       <c r="E135">
-        <v>9923</v>
+        <v>12390</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -3403,13 +3406,13 @@
         <v>138</v>
       </c>
       <c r="C136">
-        <v>12450</v>
+        <v>12837</v>
       </c>
       <c r="D136">
-        <v>145</v>
+        <v>656</v>
       </c>
       <c r="E136">
-        <v>11998</v>
+        <v>5346</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -3420,13 +3423,13 @@
         <v>139</v>
       </c>
       <c r="C137">
-        <v>12399</v>
+        <v>12803</v>
       </c>
       <c r="D137">
-        <v>316</v>
+        <v>252</v>
       </c>
       <c r="E137">
-        <v>12024</v>
+        <v>10745</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -3437,13 +3440,13 @@
         <v>140</v>
       </c>
       <c r="C138">
-        <v>11481</v>
+        <v>12641</v>
       </c>
       <c r="D138">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="E138">
-        <v>10952</v>
+        <v>11989</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -3454,13 +3457,13 @@
         <v>141</v>
       </c>
       <c r="C139">
-        <v>11398</v>
+        <v>12487</v>
       </c>
       <c r="D139">
-        <v>203</v>
+        <v>318</v>
       </c>
       <c r="E139">
-        <v>10901</v>
+        <v>12120</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -3471,13 +3474,13 @@
         <v>142</v>
       </c>
       <c r="C140">
-        <v>10530</v>
+        <v>12450</v>
       </c>
       <c r="D140">
-        <v>309</v>
+        <v>145</v>
       </c>
       <c r="E140">
-        <v>3922</v>
+        <v>11998</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -3488,13 +3491,13 @@
         <v>143</v>
       </c>
       <c r="C141">
-        <v>10085</v>
+        <v>12214</v>
       </c>
       <c r="D141">
-        <v>429</v>
+        <v>117</v>
       </c>
       <c r="E141">
-        <v>4498</v>
+        <v>9543</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -3505,13 +3508,13 @@
         <v>144</v>
       </c>
       <c r="C142">
-        <v>9768</v>
+        <v>11769</v>
       </c>
       <c r="D142">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="E142">
-        <v>8215</v>
+        <v>8247</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -3522,13 +3525,13 @@
         <v>145</v>
       </c>
       <c r="C143">
-        <v>9585</v>
+        <v>11654</v>
       </c>
       <c r="D143">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E143">
-        <v>8489</v>
+        <v>11258</v>
       </c>
     </row>
     <row r="144" spans="1:5">
@@ -3539,13 +3542,13 @@
         <v>146</v>
       </c>
       <c r="C144">
-        <v>9564</v>
+        <v>11527</v>
       </c>
       <c r="D144">
-        <v>134</v>
+        <v>263</v>
       </c>
       <c r="E144">
-        <v>7514</v>
+        <v>10015</v>
       </c>
     </row>
     <row r="145" spans="1:5">
@@ -3556,13 +3559,13 @@
         <v>147</v>
       </c>
       <c r="C145">
-        <v>9191</v>
+        <v>11254</v>
       </c>
       <c r="D145">
-        <v>367</v>
+        <v>402</v>
       </c>
       <c r="E145">
-        <v>6603</v>
+        <v>6800</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -3573,13 +3576,13 @@
         <v>148</v>
       </c>
       <c r="C146">
-        <v>9066</v>
+        <v>10707</v>
       </c>
       <c r="D146">
-        <v>176</v>
+        <v>315</v>
       </c>
       <c r="E146">
-        <v>8550</v>
+        <v>4674</v>
       </c>
     </row>
     <row r="147" spans="1:5">
@@ -3590,13 +3593,13 @@
         <v>149</v>
       </c>
       <c r="C147">
-        <v>8839</v>
+        <v>10387</v>
       </c>
       <c r="D147">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="E147">
-        <v>7193</v>
+        <v>10148</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -3607,13 +3610,13 @@
         <v>150</v>
       </c>
       <c r="C148">
-        <v>8771</v>
+        <v>10264</v>
       </c>
       <c r="D148">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="E148">
-        <v>8252</v>
+        <v>9660</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -3624,13 +3627,13 @@
         <v>151</v>
       </c>
       <c r="C149">
-        <v>8600</v>
+        <v>10084</v>
       </c>
       <c r="D149">
-        <v>181</v>
+        <v>137</v>
       </c>
       <c r="E149">
-        <v>7415</v>
+        <v>7514</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -3641,13 +3644,13 @@
         <v>152</v>
       </c>
       <c r="C150">
-        <v>7855</v>
+        <v>10077</v>
       </c>
       <c r="D150">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="E150">
-        <v>7561</v>
+        <v>8394</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -3658,13 +3661,13 @@
         <v>153</v>
       </c>
       <c r="C151">
-        <v>7751</v>
+        <v>9496</v>
       </c>
       <c r="D151">
-        <v>133</v>
+        <v>187</v>
       </c>
       <c r="E151">
-        <v>6707</v>
+        <v>8779</v>
       </c>
     </row>
     <row r="152" spans="1:5">
@@ -3675,13 +3678,13 @@
         <v>154</v>
       </c>
       <c r="C152">
-        <v>6818</v>
+        <v>9364</v>
       </c>
       <c r="D152">
-        <v>90</v>
+        <v>189</v>
       </c>
       <c r="E152">
-        <v>5552</v>
+        <v>8837</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -3692,13 +3695,13 @@
         <v>155</v>
       </c>
       <c r="C153">
-        <v>6736</v>
+        <v>8821</v>
       </c>
       <c r="D153">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="E153">
-        <v>6208</v>
+        <v>846</v>
       </c>
     </row>
     <row r="154" spans="1:5">
@@ -3709,13 +3712,13 @@
         <v>156</v>
       </c>
       <c r="C154">
-        <v>6489</v>
+        <v>8678</v>
       </c>
       <c r="D154">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="E154">
-        <v>0</v>
+        <v>7843</v>
       </c>
     </row>
     <row r="155" spans="1:5">
@@ -3726,13 +3729,13 @@
         <v>157</v>
       </c>
       <c r="C155">
-        <v>6294</v>
+        <v>7751</v>
       </c>
       <c r="D155">
-        <v>63</v>
+        <v>133</v>
       </c>
       <c r="E155">
-        <v>5854</v>
+        <v>6707</v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -3743,13 +3746,13 @@
         <v>158</v>
       </c>
       <c r="C156">
-        <v>6119</v>
+        <v>7515</v>
       </c>
       <c r="D156">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="E156">
-        <v>6035</v>
+        <v>5552</v>
       </c>
     </row>
     <row r="157" spans="1:5">
@@ -3760,13 +3763,13 @@
         <v>159</v>
       </c>
       <c r="C157">
-        <v>5997</v>
+        <v>7259</v>
       </c>
       <c r="D157">
-        <v>24</v>
+        <v>106</v>
       </c>
       <c r="E157">
-        <v>4824</v>
+        <v>6885</v>
       </c>
     </row>
     <row r="158" spans="1:5">
@@ -3777,13 +3780,13 @@
         <v>160</v>
       </c>
       <c r="C158">
-        <v>5122</v>
+        <v>6727</v>
       </c>
       <c r="D158">
-        <v>160</v>
+        <v>179</v>
       </c>
       <c r="E158">
-        <v>4686</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:5">
@@ -3794,13 +3797,13 @@
         <v>161</v>
       </c>
       <c r="C159">
-        <v>5064</v>
+        <v>6286</v>
       </c>
       <c r="D159">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="E159">
-        <v>1924</v>
+        <v>6184</v>
       </c>
     </row>
     <row r="160" spans="1:5">
@@ -3811,13 +3814,13 @@
         <v>162</v>
       </c>
       <c r="C160">
-        <v>4740</v>
+        <v>5771</v>
       </c>
       <c r="D160">
-        <v>172</v>
+        <v>39</v>
       </c>
       <c r="E160">
-        <v>4250</v>
+        <v>2416</v>
       </c>
     </row>
     <row r="161" spans="1:5">
@@ -3828,13 +3831,13 @@
         <v>163</v>
       </c>
       <c r="C161">
-        <v>4651</v>
+        <v>5728</v>
       </c>
       <c r="D161">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="E161">
-        <v>3296</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="162" spans="1:5">
@@ -3845,13 +3848,13 @@
         <v>164</v>
       </c>
       <c r="C162">
-        <v>4356</v>
+        <v>5657</v>
       </c>
       <c r="D162">
-        <v>79</v>
+        <v>1097</v>
       </c>
       <c r="E162">
-        <v>3805</v>
+        <v>2178</v>
       </c>
     </row>
     <row r="163" spans="1:5">
@@ -3862,13 +3865,13 @@
         <v>165</v>
       </c>
       <c r="C163">
-        <v>4270</v>
+        <v>5564</v>
       </c>
       <c r="D163">
-        <v>94</v>
+        <v>166</v>
       </c>
       <c r="E163">
-        <v>4148</v>
+        <v>5111</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -3879,13 +3882,13 @@
         <v>166</v>
       </c>
       <c r="C164">
-        <v>4161</v>
+        <v>4962</v>
       </c>
       <c r="D164">
-        <v>140</v>
+        <v>86</v>
       </c>
       <c r="E164">
-        <v>3607</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="165" spans="1:5">
@@ -3896,13 +3899,13 @@
         <v>167</v>
       </c>
       <c r="C165">
-        <v>4121</v>
+        <v>4765</v>
       </c>
       <c r="D165">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="E165">
-        <v>3916</v>
+        <v>4351</v>
       </c>
     </row>
     <row r="166" spans="1:5">
@@ -3913,13 +3916,13 @@
         <v>168</v>
       </c>
       <c r="C166">
-        <v>3948</v>
+        <v>4740</v>
       </c>
       <c r="D166">
-        <v>79</v>
+        <v>172</v>
       </c>
       <c r="E166">
-        <v>2791</v>
+        <v>4250</v>
       </c>
     </row>
     <row r="167" spans="1:5">
@@ -3930,13 +3933,13 @@
         <v>169</v>
       </c>
       <c r="C167">
-        <v>3913</v>
+        <v>4636</v>
       </c>
       <c r="D167">
-        <v>24</v>
+        <v>167</v>
       </c>
       <c r="E167">
-        <v>3509</v>
+        <v>4286</v>
       </c>
     </row>
     <row r="168" spans="1:5">
@@ -3947,13 +3950,13 @@
         <v>170</v>
       </c>
       <c r="C168">
-        <v>3770</v>
+        <v>4398</v>
       </c>
       <c r="D168">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="E168">
-        <v>3122</v>
+        <v>4235</v>
       </c>
     </row>
     <row r="169" spans="1:5">
@@ -3964,13 +3967,13 @@
         <v>171</v>
       </c>
       <c r="C169">
-        <v>3601</v>
+        <v>4291</v>
       </c>
       <c r="D169">
-        <v>146</v>
+        <v>94</v>
       </c>
       <c r="E169">
-        <v>3423</v>
+        <v>4181</v>
       </c>
     </row>
     <row r="170" spans="1:5">
@@ -3981,13 +3984,13 @@
         <v>172</v>
       </c>
       <c r="C170">
-        <v>3518</v>
+        <v>4016</v>
       </c>
       <c r="D170">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="E170">
-        <v>2426</v>
+        <v>2833</v>
       </c>
     </row>
     <row r="171" spans="1:5">
@@ -3998,13 +4001,13 @@
         <v>173</v>
       </c>
       <c r="C171">
-        <v>3471</v>
+        <v>3913</v>
       </c>
       <c r="D171">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="E171">
-        <v>3285</v>
+        <v>3509</v>
       </c>
     </row>
     <row r="172" spans="1:5">
@@ -4015,13 +4018,13 @@
         <v>174</v>
       </c>
       <c r="C172">
-        <v>3418</v>
+        <v>3730</v>
       </c>
       <c r="D172">
-        <v>751</v>
+        <v>44</v>
       </c>
       <c r="E172">
-        <v>1534</v>
+        <v>3607</v>
       </c>
     </row>
     <row r="173" spans="1:5">
@@ -4032,13 +4035,13 @@
         <v>175</v>
       </c>
       <c r="C173">
-        <v>3224</v>
+        <v>3678</v>
       </c>
       <c r="D173">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E173">
-        <v>3162</v>
+        <v>2426</v>
       </c>
     </row>
     <row r="174" spans="1:5">
@@ -4049,13 +4052,13 @@
         <v>176</v>
       </c>
       <c r="C174">
-        <v>3215</v>
+        <v>3601</v>
       </c>
       <c r="D174">
-        <v>281</v>
+        <v>146</v>
       </c>
       <c r="E174">
-        <v>2700</v>
+        <v>3423</v>
       </c>
     </row>
     <row r="175" spans="1:5">
@@ -4066,13 +4069,13 @@
         <v>177</v>
       </c>
       <c r="C175">
-        <v>3081</v>
+        <v>3477</v>
       </c>
       <c r="D175">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="E175">
-        <v>2591</v>
+        <v>773</v>
       </c>
     </row>
     <row r="176" spans="1:5">
@@ -4083,13 +4086,13 @@
         <v>178</v>
       </c>
       <c r="C176">
-        <v>2767</v>
+        <v>3232</v>
       </c>
       <c r="D176">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="E176">
-        <v>2653</v>
+        <v>3171</v>
       </c>
     </row>
     <row r="177" spans="1:5">
@@ -4100,13 +4103,13 @@
         <v>179</v>
       </c>
       <c r="C177">
-        <v>2658</v>
+        <v>3215</v>
       </c>
       <c r="D177">
-        <v>36</v>
+        <v>281</v>
       </c>
       <c r="E177">
-        <v>846</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="178" spans="1:5">
@@ -4117,13 +4120,13 @@
         <v>180</v>
       </c>
       <c r="C178">
-        <v>2628</v>
+        <v>3192</v>
       </c>
       <c r="D178">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="E178">
-        <v>2525</v>
+        <v>2962</v>
       </c>
     </row>
     <row r="179" spans="1:5">
@@ -4134,13 +4137,13 @@
         <v>181</v>
       </c>
       <c r="C179">
-        <v>2613</v>
+        <v>3081</v>
       </c>
       <c r="D179">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="E179">
-        <v>773</v>
+        <v>2591</v>
       </c>
     </row>
     <row r="180" spans="1:5">
@@ -4151,13 +4154,13 @@
         <v>182</v>
       </c>
       <c r="C180">
-        <v>2571</v>
+        <v>3005</v>
       </c>
       <c r="D180">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="E180">
-        <v>2198</v>
+        <v>2917</v>
       </c>
     </row>
     <row r="181" spans="1:5">
@@ -4168,13 +4171,13 @@
         <v>183</v>
       </c>
       <c r="C181">
-        <v>2395</v>
+        <v>2790</v>
       </c>
       <c r="D181">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="E181">
-        <v>337</v>
+        <v>2665</v>
       </c>
     </row>
     <row r="182" spans="1:5">
@@ -4185,13 +4188,13 @@
         <v>184</v>
       </c>
       <c r="C182">
-        <v>2326</v>
+        <v>2772</v>
       </c>
       <c r="D182">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="E182">
-        <v>1719</v>
+        <v>2475</v>
       </c>
     </row>
     <row r="183" spans="1:5">
@@ -4202,13 +4205,13 @@
         <v>185</v>
       </c>
       <c r="C183">
-        <v>2294</v>
+        <v>2395</v>
       </c>
       <c r="D183">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="E183">
-        <v>2150</v>
+        <v>337</v>
       </c>
     </row>
     <row r="184" spans="1:5">
@@ -4219,13 +4222,13 @@
         <v>186</v>
       </c>
       <c r="C184">
-        <v>2142</v>
+        <v>2369</v>
       </c>
       <c r="D184">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="E184">
-        <v>1969</v>
+        <v>2290</v>
       </c>
     </row>
     <row r="185" spans="1:5">
@@ -4236,13 +4239,13 @@
         <v>187</v>
       </c>
       <c r="C185">
-        <v>2101</v>
+        <v>2271</v>
       </c>
       <c r="D185">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="E185">
-        <v>2056</v>
+        <v>2201</v>
       </c>
     </row>
     <row r="186" spans="1:5">
@@ -4253,13 +4256,13 @@
         <v>188</v>
       </c>
       <c r="C186">
-        <v>2043</v>
+        <v>2227</v>
       </c>
       <c r="D186">
         <v>26</v>
       </c>
       <c r="E186">
-        <v>1945</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="187" spans="1:5">
@@ -4270,13 +4273,13 @@
         <v>189</v>
       </c>
       <c r="C187">
-        <v>2023</v>
+        <v>2203</v>
       </c>
       <c r="D187">
-        <v>85</v>
+        <v>27</v>
       </c>
       <c r="E187">
-        <v>1890</v>
+        <v>2142</v>
       </c>
     </row>
     <row r="188" spans="1:5">
@@ -4287,13 +4290,13 @@
         <v>190</v>
       </c>
       <c r="C188">
-        <v>1981</v>
+        <v>2042</v>
       </c>
       <c r="D188">
-        <v>26</v>
+        <v>85</v>
       </c>
       <c r="E188">
-        <v>1754</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="189" spans="1:5">
@@ -4304,13 +4307,13 @@
         <v>191</v>
       </c>
       <c r="C189">
-        <v>1808</v>
+        <v>1981</v>
       </c>
       <c r="D189">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="E189">
-        <v>1431</v>
+        <v>1754</v>
       </c>
     </row>
     <row r="190" spans="1:5">
@@ -4321,13 +4324,13 @@
         <v>192</v>
       </c>
       <c r="C190">
-        <v>1680</v>
+        <v>1935</v>
       </c>
       <c r="D190">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E190">
-        <v>950</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="191" spans="1:5">
@@ -4338,13 +4341,13 @@
         <v>193</v>
       </c>
       <c r="C191">
-        <v>1658</v>
+        <v>1808</v>
       </c>
       <c r="D191">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="E191">
-        <v>971</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="192" spans="1:5">
@@ -4355,13 +4358,13 @@
         <v>194</v>
       </c>
       <c r="C192">
-        <v>1102</v>
+        <v>1792</v>
       </c>
       <c r="D192">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E192">
-        <v>751</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="193" spans="1:5">
@@ -4372,13 +4375,13 @@
         <v>195</v>
       </c>
       <c r="C193">
-        <v>1091</v>
+        <v>1574</v>
       </c>
       <c r="D193">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E193">
-        <v>431</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="194" spans="1:5">
@@ -4389,13 +4392,13 @@
         <v>196</v>
       </c>
       <c r="C194">
-        <v>1081</v>
+        <v>1493</v>
       </c>
       <c r="D194">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E194">
-        <v>0</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="195" spans="1:5">
@@ -4406,13 +4409,13 @@
         <v>197</v>
       </c>
       <c r="C195">
-        <v>1033</v>
+        <v>1239</v>
       </c>
       <c r="D195">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="E195">
-        <v>685</v>
+        <v>644</v>
       </c>
     </row>
     <row r="196" spans="1:5">
@@ -4423,13 +4426,13 @@
         <v>198</v>
       </c>
       <c r="C196">
-        <v>1006</v>
+        <v>1209</v>
       </c>
       <c r="D196">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="E196">
-        <v>963</v>
+        <v>947</v>
       </c>
     </row>
     <row r="197" spans="1:5">
@@ -4440,13 +4443,13 @@
         <v>199</v>
       </c>
       <c r="C197">
-        <v>869</v>
+        <v>1202</v>
       </c>
       <c r="D197">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E197">
-        <v>867</v>
+        <v>865</v>
       </c>
     </row>
     <row r="198" spans="1:5">
@@ -4457,13 +4460,13 @@
         <v>200</v>
       </c>
       <c r="C198">
-        <v>821</v>
+        <v>1102</v>
       </c>
       <c r="D198">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E198">
-        <v>806</v>
+        <v>751</v>
       </c>
     </row>
     <row r="199" spans="1:5">
@@ -4474,13 +4477,13 @@
         <v>201</v>
       </c>
       <c r="C199">
-        <v>789</v>
+        <v>1081</v>
       </c>
       <c r="D199">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E199">
-        <v>709</v>
+        <v>0</v>
       </c>
     </row>
     <row r="200" spans="1:5">
@@ -4491,13 +4494,13 @@
         <v>202</v>
       </c>
       <c r="C200">
-        <v>712</v>
+        <v>1072</v>
       </c>
       <c r="D200">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E200">
-        <v>653</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="201" spans="1:5">
@@ -4508,13 +4511,13 @@
         <v>203</v>
       </c>
       <c r="C201">
-        <v>661</v>
+        <v>941</v>
       </c>
       <c r="D201">
         <v>1</v>
       </c>
       <c r="E201">
-        <v>659</v>
+        <v>876</v>
       </c>
     </row>
     <row r="202" spans="1:5">
@@ -4525,13 +4528,13 @@
         <v>204</v>
       </c>
       <c r="C202">
-        <v>641</v>
+        <v>822</v>
       </c>
       <c r="D202">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E202">
-        <v>590</v>
+        <v>807</v>
       </c>
     </row>
     <row r="203" spans="1:5">
@@ -4542,13 +4545,13 @@
         <v>205</v>
       </c>
       <c r="C203">
-        <v>492</v>
+        <v>712</v>
       </c>
       <c r="D203">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E203">
-        <v>417</v>
+        <v>653</v>
       </c>
     </row>
     <row r="204" spans="1:5">
@@ -4559,13 +4562,13 @@
         <v>206</v>
       </c>
       <c r="C204">
-        <v>475</v>
+        <v>662</v>
       </c>
       <c r="D204">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E204">
-        <v>442</v>
+        <v>660</v>
       </c>
     </row>
     <row r="205" spans="1:5">
@@ -4576,13 +4579,13 @@
         <v>207</v>
       </c>
       <c r="C205">
-        <v>326</v>
+        <v>525</v>
       </c>
       <c r="D205">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E205">
-        <v>124</v>
+        <v>499</v>
       </c>
     </row>
     <row r="206" spans="1:5">
@@ -4593,10 +4596,10 @@
         <v>208</v>
       </c>
       <c r="C206">
-        <v>302</v>
+        <v>446</v>
       </c>
       <c r="D206">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E206">
         <v>11</v>
@@ -4610,13 +4613,13 @@
         <v>209</v>
       </c>
       <c r="C207">
-        <v>205</v>
+        <v>219</v>
       </c>
       <c r="D207">
         <v>3</v>
       </c>
       <c r="E207">
-        <v>188</v>
+        <v>206</v>
       </c>
     </row>
     <row r="208" spans="1:5">
@@ -4627,13 +4630,13 @@
         <v>210</v>
       </c>
       <c r="C208">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="D208">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E208">
-        <v>32</v>
+        <v>161</v>
       </c>
     </row>
     <row r="209" spans="1:5">
@@ -4644,13 +4647,13 @@
         <v>211</v>
       </c>
       <c r="C209">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="D209">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E209">
-        <v>141</v>
+        <v>32</v>
       </c>
     </row>
     <row r="210" spans="1:5">
@@ -4661,13 +4664,13 @@
         <v>212</v>
       </c>
       <c r="C210">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="D210">
         <v>1</v>
       </c>
       <c r="E210">
-        <v>131</v>
+        <v>154</v>
       </c>
     </row>
     <row r="211" spans="1:5">
@@ -4678,13 +4681,13 @@
         <v>213</v>
       </c>
       <c r="C211">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="D211">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E211">
-        <v>148</v>
+        <v>131</v>
       </c>
     </row>
     <row r="212" spans="1:5">
@@ -4698,10 +4701,10 @@
         <v>148</v>
       </c>
       <c r="D212">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E212">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="213" spans="1:5">
@@ -4729,7 +4732,7 @@
         <v>216</v>
       </c>
       <c r="C214">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D214">
         <v>0</v>
@@ -4746,13 +4749,13 @@
         <v>217</v>
       </c>
       <c r="C215">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D215">
         <v>2</v>
       </c>
       <c r="E215">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="216" spans="1:5">
@@ -4763,13 +4766,13 @@
         <v>218</v>
       </c>
       <c r="C216">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D216">
         <v>0</v>
       </c>
       <c r="E216">
-        <v>0</v>
+        <v>55</v>
       </c>
     </row>
     <row r="217" spans="1:5">
@@ -4780,13 +4783,13 @@
         <v>219</v>
       </c>
       <c r="C217">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D217">
         <v>0</v>
       </c>
       <c r="E217">
-        <v>54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="218" spans="1:5">
@@ -4797,13 +4800,13 @@
         <v>220</v>
       </c>
       <c r="C218">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D218">
         <v>0</v>
       </c>
       <c r="E218">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="219" spans="1:5">
@@ -4814,13 +4817,13 @@
         <v>221</v>
       </c>
       <c r="C219">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D219">
         <v>0</v>
       </c>
       <c r="E219">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="220" spans="1:5">
@@ -4837,7 +4840,7 @@
         <v>0</v>
       </c>
       <c r="E220">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="221" spans="1:5">
@@ -4899,13 +4902,13 @@
         <v>226</v>
       </c>
       <c r="C224">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D224">
         <v>0</v>
       </c>
       <c r="E224">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="225" spans="1:5">
@@ -4916,13 +4919,13 @@
         <v>227</v>
       </c>
       <c r="C225">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D225">
         <v>0</v>
       </c>
       <c r="E225">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="226" spans="1:5">
@@ -4967,13 +4970,13 @@
         <v>230</v>
       </c>
       <c r="C228">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D228">
         <v>0</v>
       </c>
       <c r="E228">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="229" spans="1:5">
@@ -5069,13 +5072,13 @@
         <v>236</v>
       </c>
       <c r="C234">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D234">
         <v>0</v>
       </c>
       <c r="E234">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="235" spans="1:5">
@@ -5092,7 +5095,7 @@
         <v>0</v>
       </c>
       <c r="E235">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="236" spans="1:5">
@@ -5109,7 +5112,7 @@
         <v>0</v>
       </c>
       <c r="E236">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="237" spans="1:5">
@@ -5120,13 +5123,13 @@
         <v>239</v>
       </c>
       <c r="C237">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D237">
         <v>0</v>
       </c>
       <c r="E237">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="238" spans="1:5">
@@ -5137,7 +5140,7 @@
         <v>240</v>
       </c>
       <c r="C238">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D238">
         <v>0</v>
@@ -5154,12 +5157,29 @@
         <v>241</v>
       </c>
       <c r="C239">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D239">
         <v>0</v>
       </c>
       <c r="E239">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5">
+      <c r="A240" s="1">
+        <v>238</v>
+      </c>
+      <c r="B240" t="s">
+        <v>242</v>
+      </c>
+      <c r="C240">
+        <v>0</v>
+      </c>
+      <c r="D240">
+        <v>0</v>
+      </c>
+      <c r="E240">
         <v>0</v>
       </c>
     </row>

</xml_diff>